<commit_message>
Update Neutral and NeutralUnits in CardPool
</commit_message>
<xml_diff>
--- a/Resources/CardPoolDatabase.xlsx
+++ b/Resources/CardPoolDatabase.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="208">
   <si>
     <t>Name</t>
   </si>
@@ -340,11 +340,423 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PicDir</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cardID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vampire: Ekimmara</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vampire Ekimmara.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Who would think overgrown bats would have a tatse for gaudy jewelry?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Muster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vampire: Fleder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vampire Fleder.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Muster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vampire: Garkain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vampire Garkain.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blood-drinkers and corpse-eaters so foul their very ugliness paralyses foes.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vampire: Katakan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vampire Katakan.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Drinking blood of the Continent since the Conjunction.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Muster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Werewolf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wolves aren't as bad as they say.  Werewolves, though - they're worse.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wyvern</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Imagin a cross between a winged snake and a nightmare.  Wyverns are worse.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RangedCombat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Higher vampires embrace their victims.  Fleders rip them to shreds.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cirilla Finoa Elen Riannon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cirilla Finoa Elen Riannon 2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Know when fairy tales cease to be tales?  When people start believing in them.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Neutral</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hero</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dandelion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dandelion 2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dandelion, you're a cynic, a lecher, a whoremonger, a liar - and my best friend.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Neutral</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UnitHorn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emiel Regis Rohellec Terzieff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emiel Regis Rohellec Terzieff 2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Men, the polite ones, at least, would call me a monster.  A blood-drinking freak.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gaunter O'Dimm: Darkness</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gaunter O'Dimm Darkness 1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fear not the shadows, but the light.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Muster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Geralt of Rivia</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Geralt of Rivia 2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If that's what it takes to save the world, it's better to let that world die.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hero</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mysterious Elf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mysterious Elf 2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>You humans have... Unusual tastes.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hero</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Triss Merigold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Triss Merigold 2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I can take care of myself.  Trust me.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vesemir</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vesemir 2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If you're to be hanged, ask for water.  Anything can happen before they fetch it.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ordinary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Villentretenmerth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Villentretenmerth 2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Also calls himself Borkh Three Jackdaws... he's not the best at names.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UnitScorch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yennefer of Vengerberg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yennefer of Vengerberg 2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Magic is Chaos, Art and Science.  It is a curse, ablessing and a progression.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zoltan Chivay</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zoltan Chivay 2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Life without old mates and booze is like a woman without a rump.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ordinary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NullULevel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spell</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biting Frost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biting Frost 1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Best part about frost - bodies of the fallen don't rot so quickly.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NullUType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weather</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BitingFrost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BitingFrost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clear Weather</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clear Weather 1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The sun's shinin.  Dromle!  The sun's shinin'!  Maybe there's hope left after all.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ClearWeather</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Impenetrablr Fog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Impenetrablr Fog 1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A good commander's dream... a bad one's horror.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Torrential Rain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Torrential Rain 1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Even the rain in the land smells like piss.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commander's Horn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commander's Horn 1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plus one to morale, minus three to hearing.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Horn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpellHorn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Decoy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Decoy 1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>When you run out of peasants, decoys also make decent arrow fodder.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Decoy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Decoy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scorch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scorch 1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pillars of flame turn the mightiest to ash.  All others tremble in shock and awe.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scorch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpellScorch</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -714,32 +1126,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q102"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="38.125" customWidth="1"/>
-    <col min="3" max="3" width="37.125" customWidth="1"/>
-    <col min="4" max="4" width="71.5" customWidth="1"/>
+    <col min="2" max="2" width="14.625" customWidth="1"/>
+    <col min="3" max="3" width="10.25" customWidth="1"/>
+    <col min="4" max="4" width="11.25" customWidth="1"/>
     <col min="5" max="5" width="2.5" customWidth="1"/>
     <col min="6" max="6" width="6.625" customWidth="1"/>
-    <col min="8" max="8" width="19.375" customWidth="1"/>
-    <col min="9" max="9" width="19.625" customWidth="1"/>
+    <col min="7" max="7" width="4.625" customWidth="1"/>
+    <col min="8" max="8" width="3.375" customWidth="1"/>
+    <col min="9" max="9" width="9.375" customWidth="1"/>
     <col min="10" max="10" width="7.625" customWidth="1"/>
-    <col min="11" max="11" width="9" customWidth="1"/>
-    <col min="12" max="12" width="9.5" customWidth="1"/>
-    <col min="13" max="13" width="16.25" customWidth="1"/>
+    <col min="11" max="11" width="5.375" customWidth="1"/>
+    <col min="12" max="12" width="5.75" customWidth="1"/>
+    <col min="13" max="13" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -2232,6 +2647,15 @@
       <c r="A36">
         <v>34</v>
       </c>
+      <c r="B36" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" t="s">
+        <v>106</v>
+      </c>
       <c r="E36">
         <v>1</v>
       </c>
@@ -2242,7 +2666,7 @@
         <v>15</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I36" t="s">
         <v>16</v>
@@ -2257,7 +2681,7 @@
         <v>19</v>
       </c>
       <c r="M36" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="N36" t="b">
         <v>0</v>
@@ -2267,6 +2691,15 @@
       <c r="A37">
         <v>35</v>
       </c>
+      <c r="B37" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" t="s">
+        <v>124</v>
+      </c>
       <c r="E37">
         <v>1</v>
       </c>
@@ -2277,7 +2710,7 @@
         <v>15</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I37" t="s">
         <v>16</v>
@@ -2292,7 +2725,7 @@
         <v>19</v>
       </c>
       <c r="M37" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="N37" t="b">
         <v>0</v>
@@ -2302,6 +2735,15 @@
       <c r="A38">
         <v>36</v>
       </c>
+      <c r="B38" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" t="s">
+        <v>113</v>
+      </c>
       <c r="E38">
         <v>1</v>
       </c>
@@ -2312,7 +2754,7 @@
         <v>15</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I38" t="s">
         <v>16</v>
@@ -2327,7 +2769,7 @@
         <v>19</v>
       </c>
       <c r="M38" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="N38" t="b">
         <v>0</v>
@@ -2337,6 +2779,15 @@
       <c r="A39">
         <v>37</v>
       </c>
+      <c r="B39" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" t="s">
+        <v>117</v>
+      </c>
       <c r="E39">
         <v>1</v>
       </c>
@@ -2347,7 +2798,7 @@
         <v>15</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I39" t="s">
         <v>16</v>
@@ -2362,7 +2813,7 @@
         <v>19</v>
       </c>
       <c r="M39" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="N39" t="b">
         <v>0</v>
@@ -2372,6 +2823,12 @@
       <c r="A40">
         <v>38</v>
       </c>
+      <c r="B40" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" t="s">
+        <v>120</v>
+      </c>
       <c r="E40">
         <v>1</v>
       </c>
@@ -2382,7 +2839,7 @@
         <v>15</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I40" t="s">
         <v>16</v>
@@ -2407,6 +2864,12 @@
       <c r="A41">
         <v>39</v>
       </c>
+      <c r="B41" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" t="s">
+        <v>122</v>
+      </c>
       <c r="E41">
         <v>1</v>
       </c>
@@ -2417,10 +2880,10 @@
         <v>15</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I41" t="s">
-        <v>16</v>
+        <v>123</v>
       </c>
       <c r="J41" t="s">
         <v>17</v>
@@ -2442,6 +2905,15 @@
       <c r="A42">
         <v>40</v>
       </c>
+      <c r="B42" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" t="s">
+        <v>126</v>
+      </c>
+      <c r="D42" t="s">
+        <v>127</v>
+      </c>
       <c r="E42">
         <v>1</v>
       </c>
@@ -2449,16 +2921,16 @@
         <v>14</v>
       </c>
       <c r="G42" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I42" t="s">
         <v>16</v>
       </c>
       <c r="J42" t="s">
-        <v>17</v>
+        <v>129</v>
       </c>
       <c r="K42" t="s">
         <v>18</v>
@@ -2477,6 +2949,15 @@
       <c r="A43">
         <v>41</v>
       </c>
+      <c r="B43" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" t="s">
+        <v>131</v>
+      </c>
+      <c r="D43" t="s">
+        <v>132</v>
+      </c>
       <c r="E43">
         <v>1</v>
       </c>
@@ -2484,10 +2965,10 @@
         <v>14</v>
       </c>
       <c r="G43" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I43" t="s">
         <v>16</v>
@@ -2502,7 +2983,7 @@
         <v>19</v>
       </c>
       <c r="M43" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="N43" t="b">
         <v>0</v>
@@ -2512,6 +2993,15 @@
       <c r="A44">
         <v>42</v>
       </c>
+      <c r="B44" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" t="s">
+        <v>136</v>
+      </c>
+      <c r="D44" t="s">
+        <v>137</v>
+      </c>
       <c r="E44">
         <v>1</v>
       </c>
@@ -2519,10 +3009,10 @@
         <v>14</v>
       </c>
       <c r="G44" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I44" t="s">
         <v>16</v>
@@ -2547,20 +3037,29 @@
       <c r="A45">
         <v>43</v>
       </c>
+      <c r="B45" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" t="s">
+        <v>139</v>
+      </c>
+      <c r="D45" t="s">
+        <v>140</v>
+      </c>
       <c r="E45">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G45" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I45" t="s">
-        <v>16</v>
+        <v>123</v>
       </c>
       <c r="J45" t="s">
         <v>17</v>
@@ -2572,7 +3071,7 @@
         <v>19</v>
       </c>
       <c r="M45" t="s">
-        <v>102</v>
+        <v>141</v>
       </c>
       <c r="N45" t="b">
         <v>0</v>
@@ -2582,6 +3081,15 @@
       <c r="A46">
         <v>44</v>
       </c>
+      <c r="B46" t="s">
+        <v>142</v>
+      </c>
+      <c r="C46" t="s">
+        <v>143</v>
+      </c>
+      <c r="D46" t="s">
+        <v>144</v>
+      </c>
       <c r="E46">
         <v>1</v>
       </c>
@@ -2589,16 +3097,16 @@
         <v>14</v>
       </c>
       <c r="G46" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I46" t="s">
         <v>16</v>
       </c>
       <c r="J46" t="s">
-        <v>17</v>
+        <v>145</v>
       </c>
       <c r="K46" t="s">
         <v>18</v>
@@ -2617,6 +3125,15 @@
       <c r="A47">
         <v>45</v>
       </c>
+      <c r="B47" t="s">
+        <v>146</v>
+      </c>
+      <c r="C47" t="s">
+        <v>147</v>
+      </c>
+      <c r="D47" t="s">
+        <v>148</v>
+      </c>
       <c r="E47">
         <v>1</v>
       </c>
@@ -2624,7 +3141,7 @@
         <v>14</v>
       </c>
       <c r="G47" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -2633,7 +3150,7 @@
         <v>16</v>
       </c>
       <c r="J47" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="K47" t="s">
         <v>18</v>
@@ -2642,7 +3159,7 @@
         <v>19</v>
       </c>
       <c r="M47" t="s">
-        <v>102</v>
+        <v>150</v>
       </c>
       <c r="N47" t="b">
         <v>0</v>
@@ -2652,163 +3169,638 @@
       <c r="A48">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>151</v>
+      </c>
+      <c r="C48" t="s">
+        <v>152</v>
+      </c>
+      <c r="D48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" t="s">
+        <v>133</v>
+      </c>
+      <c r="H48">
+        <v>7</v>
+      </c>
+      <c r="I48" t="s">
+        <v>16</v>
+      </c>
+      <c r="J48" t="s">
+        <v>149</v>
+      </c>
+      <c r="K48" t="s">
+        <v>18</v>
+      </c>
+      <c r="L48" t="s">
+        <v>19</v>
+      </c>
+      <c r="M48" t="s">
+        <v>102</v>
+      </c>
+      <c r="N48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>154</v>
+      </c>
+      <c r="C49" t="s">
+        <v>155</v>
+      </c>
+      <c r="D49" t="s">
+        <v>156</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G49" t="s">
+        <v>133</v>
+      </c>
+      <c r="H49">
+        <v>6</v>
+      </c>
+      <c r="I49" t="s">
+        <v>16</v>
+      </c>
+      <c r="J49" t="s">
+        <v>157</v>
+      </c>
+      <c r="K49" t="s">
+        <v>18</v>
+      </c>
+      <c r="L49" t="s">
+        <v>19</v>
+      </c>
+      <c r="M49" t="s">
+        <v>102</v>
+      </c>
+      <c r="N49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>158</v>
+      </c>
+      <c r="C50" t="s">
+        <v>159</v>
+      </c>
+      <c r="D50" t="s">
+        <v>160</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" t="s">
+        <v>133</v>
+      </c>
+      <c r="H50">
+        <v>7</v>
+      </c>
+      <c r="I50" t="s">
+        <v>16</v>
+      </c>
+      <c r="J50" t="s">
+        <v>157</v>
+      </c>
+      <c r="K50" t="s">
+        <v>18</v>
+      </c>
+      <c r="L50" t="s">
+        <v>19</v>
+      </c>
+      <c r="M50" t="s">
+        <v>161</v>
+      </c>
+      <c r="N50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>162</v>
+      </c>
+      <c r="C51" t="s">
+        <v>163</v>
+      </c>
+      <c r="D51" t="s">
+        <v>164</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G51" t="s">
+        <v>133</v>
+      </c>
+      <c r="H51">
+        <v>7</v>
+      </c>
+      <c r="I51" t="s">
+        <v>123</v>
+      </c>
+      <c r="J51" t="s">
+        <v>149</v>
+      </c>
+      <c r="K51" t="s">
+        <v>18</v>
+      </c>
+      <c r="L51" t="s">
+        <v>19</v>
+      </c>
+      <c r="M51" t="s">
+        <v>165</v>
+      </c>
+      <c r="N51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" t="s">
+        <v>167</v>
+      </c>
+      <c r="D52" t="s">
+        <v>168</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G52" t="s">
+        <v>133</v>
+      </c>
+      <c r="H52">
+        <v>5</v>
+      </c>
+      <c r="I52" t="s">
+        <v>16</v>
+      </c>
+      <c r="J52" t="s">
+        <v>169</v>
+      </c>
+      <c r="K52" t="s">
+        <v>18</v>
+      </c>
+      <c r="L52" t="s">
+        <v>19</v>
+      </c>
+      <c r="M52" t="s">
+        <v>102</v>
+      </c>
+      <c r="N52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>172</v>
+      </c>
+      <c r="C53" t="s">
+        <v>173</v>
+      </c>
+      <c r="D53" t="s">
+        <v>174</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G53" t="s">
+        <v>133</v>
+      </c>
+      <c r="H53">
+        <v>-1</v>
+      </c>
+      <c r="I53" t="s">
+        <v>175</v>
+      </c>
+      <c r="J53" t="s">
+        <v>170</v>
+      </c>
+      <c r="K53" t="s">
+        <v>176</v>
+      </c>
+      <c r="L53" t="s">
+        <v>177</v>
+      </c>
+      <c r="M53" t="s">
+        <v>178</v>
+      </c>
+      <c r="N53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>179</v>
+      </c>
+      <c r="C54" t="s">
+        <v>180</v>
+      </c>
+      <c r="D54" t="s">
+        <v>181</v>
+      </c>
+      <c r="E54">
+        <v>3</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G54" t="s">
+        <v>133</v>
+      </c>
+      <c r="H54">
+        <v>-1</v>
+      </c>
+      <c r="I54" t="s">
+        <v>175</v>
+      </c>
+      <c r="J54" t="s">
+        <v>170</v>
+      </c>
+      <c r="K54" t="s">
+        <v>176</v>
+      </c>
+      <c r="L54" t="s">
+        <v>182</v>
+      </c>
+      <c r="M54" t="s">
+        <v>182</v>
+      </c>
+      <c r="N54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>183</v>
+      </c>
+      <c r="C55" t="s">
+        <v>184</v>
+      </c>
+      <c r="D55" t="s">
+        <v>185</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G55" t="s">
+        <v>133</v>
+      </c>
+      <c r="H55">
+        <v>-1</v>
+      </c>
+      <c r="I55" t="s">
+        <v>175</v>
+      </c>
+      <c r="J55" t="s">
+        <v>170</v>
+      </c>
+      <c r="K55" t="s">
+        <v>176</v>
+      </c>
+      <c r="L55" t="s">
+        <v>186</v>
+      </c>
+      <c r="M55" t="s">
+        <v>187</v>
+      </c>
+      <c r="N55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>188</v>
+      </c>
+      <c r="C56" t="s">
+        <v>189</v>
+      </c>
+      <c r="D56" t="s">
+        <v>190</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G56" t="s">
+        <v>133</v>
+      </c>
+      <c r="H56">
+        <v>-1</v>
+      </c>
+      <c r="I56" t="s">
+        <v>175</v>
+      </c>
+      <c r="J56" t="s">
+        <v>170</v>
+      </c>
+      <c r="K56" t="s">
+        <v>176</v>
+      </c>
+      <c r="L56" t="s">
+        <v>191</v>
+      </c>
+      <c r="M56" t="s">
+        <v>192</v>
+      </c>
+      <c r="N56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>193</v>
+      </c>
+      <c r="C57" t="s">
+        <v>194</v>
+      </c>
+      <c r="D57" t="s">
+        <v>195</v>
+      </c>
+      <c r="E57">
+        <v>3</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G57" t="s">
+        <v>133</v>
+      </c>
+      <c r="H57">
+        <v>-1</v>
+      </c>
+      <c r="I57" t="s">
+        <v>175</v>
+      </c>
+      <c r="J57" t="s">
+        <v>170</v>
+      </c>
+      <c r="K57" t="s">
+        <v>196</v>
+      </c>
+      <c r="L57" t="s">
+        <v>19</v>
+      </c>
+      <c r="M57" t="s">
+        <v>197</v>
+      </c>
+      <c r="N57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>198</v>
+      </c>
+      <c r="C58" t="s">
+        <v>199</v>
+      </c>
+      <c r="D58" t="s">
+        <v>200</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G58" t="s">
+        <v>133</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58" t="s">
+        <v>175</v>
+      </c>
+      <c r="J58" t="s">
+        <v>170</v>
+      </c>
+      <c r="K58" t="s">
+        <v>201</v>
+      </c>
+      <c r="L58" t="s">
+        <v>19</v>
+      </c>
+      <c r="M58" t="s">
+        <v>202</v>
+      </c>
+      <c r="N58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>203</v>
+      </c>
+      <c r="C59" t="s">
+        <v>204</v>
+      </c>
+      <c r="D59" t="s">
+        <v>205</v>
+      </c>
+      <c r="E59">
+        <v>3</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G59" t="s">
+        <v>133</v>
+      </c>
+      <c r="H59">
+        <v>-1</v>
+      </c>
+      <c r="I59" t="s">
+        <v>175</v>
+      </c>
+      <c r="J59" t="s">
+        <v>170</v>
+      </c>
+      <c r="K59" t="s">
+        <v>206</v>
+      </c>
+      <c r="L59" t="s">
+        <v>19</v>
+      </c>
+      <c r="M59" t="s">
+        <v>207</v>
+      </c>
+      <c r="N59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F65" s="1"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F66" s="1"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
add python file which can transfer excel file to Json file.
</commit_message>
<xml_diff>
--- a/Resources/CardPoolDatabase.xlsx
+++ b/Resources/CardPoolDatabase.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Junce\Source\Repos\GwentCore\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cpp\GwentCore\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -764,6 +764,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0_ "/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -803,11 +806,23 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1126,28 +1141,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C179" sqref="C179"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="9" style="2"/>
     <col min="2" max="2" width="14.625" customWidth="1"/>
     <col min="3" max="3" width="10.25" customWidth="1"/>
     <col min="4" max="4" width="11.25" customWidth="1"/>
-    <col min="5" max="5" width="2.5" customWidth="1"/>
+    <col min="5" max="5" width="2.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="6.625" customWidth="1"/>
     <col min="7" max="7" width="4.625" customWidth="1"/>
-    <col min="8" max="8" width="3.375" customWidth="1"/>
+    <col min="8" max="8" width="3.375" style="2" customWidth="1"/>
     <col min="9" max="9" width="9.375" customWidth="1"/>
     <col min="10" max="10" width="7.625" customWidth="1"/>
     <col min="11" max="11" width="5.375" customWidth="1"/>
     <col min="12" max="12" width="5.75" customWidth="1"/>
     <col min="13" max="13" width="12.5" customWidth="1"/>
+    <col min="14" max="14" width="9" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B1" t="s">
@@ -1159,7 +1176,7 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
@@ -1168,7 +1185,7 @@
       <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I1" t="s">
@@ -1186,12 +1203,12 @@
       <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="4" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -1203,7 +1220,7 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
@@ -1212,7 +1229,7 @@
       <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <v>4</v>
       </c>
       <c r="I2" t="s">
@@ -1230,12 +1247,12 @@
       <c r="M2" t="s">
         <v>20</v>
       </c>
-      <c r="N2" t="b">
+      <c r="N2" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -1247,7 +1264,7 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>1</v>
       </c>
       <c r="F3" t="s">
@@ -1256,7 +1273,7 @@
       <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <v>4</v>
       </c>
       <c r="I3" t="s">
@@ -1274,12 +1291,12 @@
       <c r="M3" t="s">
         <v>20</v>
       </c>
-      <c r="N3" t="b">
+      <c r="N3" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -1291,7 +1308,7 @@
       <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>1</v>
       </c>
       <c r="F4" t="s">
@@ -1300,7 +1317,7 @@
       <c r="G4" t="s">
         <v>15</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <v>4</v>
       </c>
       <c r="I4" t="s">
@@ -1318,12 +1335,12 @@
       <c r="M4" t="s">
         <v>20</v>
       </c>
-      <c r="N4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="N4" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -1335,7 +1352,7 @@
       <c r="D5" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="3">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -1344,7 +1361,7 @@
       <c r="G5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="3">
         <v>6</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -1362,14 +1379,14 @@
       <c r="M5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="1" t="b">
+      <c r="N5" s="5" t="b">
         <v>0</v>
       </c>
       <c r="O5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -1381,7 +1398,7 @@
       <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>1</v>
       </c>
       <c r="F6" t="s">
@@ -1390,7 +1407,7 @@
       <c r="G6" t="s">
         <v>15</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <v>4</v>
       </c>
       <c r="I6" t="s">
@@ -1408,12 +1425,12 @@
       <c r="M6" t="s">
         <v>29</v>
       </c>
-      <c r="N6" t="b">
+      <c r="N6" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -1425,7 +1442,7 @@
       <c r="D7" t="s">
         <v>32</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>1</v>
       </c>
       <c r="F7" t="s">
@@ -1434,7 +1451,7 @@
       <c r="G7" t="s">
         <v>15</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <v>2</v>
       </c>
       <c r="I7" t="s">
@@ -1452,12 +1469,12 @@
       <c r="M7" t="s">
         <v>34</v>
       </c>
-      <c r="N7" t="b">
+      <c r="N7" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -1469,7 +1486,7 @@
       <c r="D8" t="s">
         <v>37</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>1</v>
       </c>
       <c r="F8" t="s">
@@ -1478,7 +1495,7 @@
       <c r="G8" t="s">
         <v>15</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="2">
         <v>2</v>
       </c>
       <c r="I8" t="s">
@@ -1496,12 +1513,12 @@
       <c r="M8" t="s">
         <v>29</v>
       </c>
-      <c r="N8" t="b">
+      <c r="N8" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" t="s">
@@ -1513,7 +1530,7 @@
       <c r="D9" t="s">
         <v>93</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>1</v>
       </c>
       <c r="F9" t="s">
@@ -1522,7 +1539,7 @@
       <c r="G9" t="s">
         <v>15</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <v>6</v>
       </c>
       <c r="I9" t="s">
@@ -1540,12 +1557,12 @@
       <c r="M9" t="s">
         <v>20</v>
       </c>
-      <c r="N9" t="b">
+      <c r="N9" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" t="s">
@@ -1557,7 +1574,7 @@
       <c r="D10" t="s">
         <v>43</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>1</v>
       </c>
       <c r="F10" t="s">
@@ -1566,7 +1583,7 @@
       <c r="G10" t="s">
         <v>15</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="2">
         <v>6</v>
       </c>
       <c r="I10" t="s">
@@ -1584,12 +1601,12 @@
       <c r="M10" t="s">
         <v>20</v>
       </c>
-      <c r="N10" t="b">
+      <c r="N10" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" t="s">
@@ -1601,7 +1618,7 @@
       <c r="D11" t="s">
         <v>46</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>1</v>
       </c>
       <c r="F11" t="s">
@@ -1610,7 +1627,7 @@
       <c r="G11" t="s">
         <v>15</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <v>6</v>
       </c>
       <c r="I11" t="s">
@@ -1628,12 +1645,12 @@
       <c r="M11" t="s">
         <v>20</v>
       </c>
-      <c r="N11" t="b">
+      <c r="N11" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12" t="s">
@@ -1645,7 +1662,7 @@
       <c r="D12" t="s">
         <v>49</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>1</v>
       </c>
       <c r="F12" t="s">
@@ -1654,7 +1671,7 @@
       <c r="G12" t="s">
         <v>15</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="2">
         <v>10</v>
       </c>
       <c r="I12" t="s">
@@ -1672,12 +1689,12 @@
       <c r="M12" t="s">
         <v>29</v>
       </c>
-      <c r="N12" t="b">
+      <c r="N12" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
       <c r="B13" t="s">
@@ -1689,7 +1706,7 @@
       <c r="D13" t="s">
         <v>53</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>1</v>
       </c>
       <c r="F13" t="s">
@@ -1698,7 +1715,7 @@
       <c r="G13" t="s">
         <v>15</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="2">
         <v>6</v>
       </c>
       <c r="I13" t="s">
@@ -1716,12 +1733,12 @@
       <c r="M13" t="s">
         <v>29</v>
       </c>
-      <c r="N13" t="b">
+      <c r="N13" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="2">
         <v>12</v>
       </c>
       <c r="B14" t="s">
@@ -1730,7 +1747,7 @@
       <c r="D14" t="s">
         <v>94</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>1</v>
       </c>
       <c r="F14" t="s">
@@ -1739,7 +1756,7 @@
       <c r="G14" t="s">
         <v>15</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="2">
         <v>2</v>
       </c>
       <c r="I14" t="s">
@@ -1757,12 +1774,12 @@
       <c r="M14" t="s">
         <v>29</v>
       </c>
-      <c r="N14" t="b">
+      <c r="N14" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="2">
         <v>13</v>
       </c>
       <c r="B15" t="s">
@@ -1771,7 +1788,7 @@
       <c r="D15" t="s">
         <v>95</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>1</v>
       </c>
       <c r="F15" t="s">
@@ -1780,7 +1797,7 @@
       <c r="G15" t="s">
         <v>15</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="2">
         <v>6</v>
       </c>
       <c r="I15" t="s">
@@ -1798,12 +1815,12 @@
       <c r="M15" t="s">
         <v>29</v>
       </c>
-      <c r="N15" t="b">
+      <c r="N15" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="2">
         <v>14</v>
       </c>
       <c r="B16" t="s">
@@ -1812,7 +1829,7 @@
       <c r="D16" t="s">
         <v>57</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>1</v>
       </c>
       <c r="F16" t="s">
@@ -1821,7 +1838,7 @@
       <c r="G16" t="s">
         <v>15</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="2">
         <v>6</v>
       </c>
       <c r="I16" t="s">
@@ -1839,12 +1856,12 @@
       <c r="M16" t="s">
         <v>29</v>
       </c>
-      <c r="N16" t="b">
+      <c r="N16" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="2">
         <v>15</v>
       </c>
       <c r="B17" t="s">
@@ -1853,7 +1870,7 @@
       <c r="D17" t="s">
         <v>59</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>1</v>
       </c>
       <c r="F17" t="s">
@@ -1862,7 +1879,7 @@
       <c r="G17" t="s">
         <v>15</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="2">
         <v>2</v>
       </c>
       <c r="I17" t="s">
@@ -1880,12 +1897,12 @@
       <c r="M17" t="s">
         <v>29</v>
       </c>
-      <c r="N17" t="b">
+      <c r="N17" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="2">
         <v>16</v>
       </c>
       <c r="B18" t="s">
@@ -1894,7 +1911,7 @@
       <c r="D18" t="s">
         <v>61</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>1</v>
       </c>
       <c r="F18" t="s">
@@ -1903,7 +1920,7 @@
       <c r="G18" t="s">
         <v>15</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="2">
         <v>5</v>
       </c>
       <c r="I18" t="s">
@@ -1921,12 +1938,12 @@
       <c r="M18" t="s">
         <v>29</v>
       </c>
-      <c r="N18" t="b">
+      <c r="N18" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="A19" s="2">
         <v>17</v>
       </c>
       <c r="B19" t="s">
@@ -1935,7 +1952,7 @@
       <c r="D19" t="s">
         <v>96</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>1</v>
       </c>
       <c r="F19" t="s">
@@ -1944,7 +1961,7 @@
       <c r="G19" t="s">
         <v>15</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="2">
         <v>5</v>
       </c>
       <c r="I19" t="s">
@@ -1962,12 +1979,12 @@
       <c r="M19" t="s">
         <v>29</v>
       </c>
-      <c r="N19" t="b">
+      <c r="N19" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" s="2">
         <v>18</v>
       </c>
       <c r="B20" t="s">
@@ -1976,7 +1993,7 @@
       <c r="D20" t="s">
         <v>97</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>1</v>
       </c>
       <c r="F20" t="s">
@@ -1985,7 +2002,7 @@
       <c r="G20" t="s">
         <v>15</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="2">
         <v>2</v>
       </c>
       <c r="I20" t="s">
@@ -2003,12 +2020,12 @@
       <c r="M20" t="s">
         <v>29</v>
       </c>
-      <c r="N20" t="b">
+      <c r="N20" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="2">
         <v>19</v>
       </c>
       <c r="B21" t="s">
@@ -2020,7 +2037,7 @@
       <c r="D21" t="s">
         <v>66</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>1</v>
       </c>
       <c r="F21" t="s">
@@ -2029,7 +2046,7 @@
       <c r="G21" t="s">
         <v>15</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="2">
         <v>1</v>
       </c>
       <c r="I21" t="s">
@@ -2047,12 +2064,12 @@
       <c r="M21" t="s">
         <v>20</v>
       </c>
-      <c r="N21" t="b">
+      <c r="N21" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="A22" s="2">
         <v>20</v>
       </c>
       <c r="B22" t="s">
@@ -2064,7 +2081,7 @@
       <c r="D22" t="s">
         <v>66</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>1</v>
       </c>
       <c r="F22" t="s">
@@ -2073,7 +2090,7 @@
       <c r="G22" t="s">
         <v>15</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="2">
         <v>1</v>
       </c>
       <c r="I22" t="s">
@@ -2091,12 +2108,12 @@
       <c r="M22" t="s">
         <v>20</v>
       </c>
-      <c r="N22" t="b">
+      <c r="N22" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="2">
         <v>21</v>
       </c>
       <c r="B23" t="s">
@@ -2108,7 +2125,7 @@
       <c r="D23" t="s">
         <v>66</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <v>1</v>
       </c>
       <c r="F23" t="s">
@@ -2117,7 +2134,7 @@
       <c r="G23" t="s">
         <v>15</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="2">
         <v>1</v>
       </c>
       <c r="I23" t="s">
@@ -2135,12 +2152,12 @@
       <c r="M23" t="s">
         <v>20</v>
       </c>
-      <c r="N23" t="b">
+      <c r="N23" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" s="2">
         <v>22</v>
       </c>
       <c r="B24" t="s">
@@ -2149,7 +2166,7 @@
       <c r="D24" t="s">
         <v>70</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>1</v>
       </c>
       <c r="F24" t="s">
@@ -2158,7 +2175,7 @@
       <c r="G24" t="s">
         <v>15</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="2">
         <v>5</v>
       </c>
       <c r="I24" t="s">
@@ -2176,12 +2193,12 @@
       <c r="M24" t="s">
         <v>29</v>
       </c>
-      <c r="N24" t="b">
+      <c r="N24" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="2">
         <v>23</v>
       </c>
       <c r="B25" t="s">
@@ -2190,7 +2207,7 @@
       <c r="D25" t="s">
         <v>98</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <v>1</v>
       </c>
       <c r="F25" t="s">
@@ -2199,7 +2216,7 @@
       <c r="G25" t="s">
         <v>15</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="2">
         <v>5</v>
       </c>
       <c r="I25" t="s">
@@ -2217,12 +2234,12 @@
       <c r="M25" t="s">
         <v>29</v>
       </c>
-      <c r="N25" t="b">
+      <c r="N25" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="2">
         <v>24</v>
       </c>
       <c r="B26" t="s">
@@ -2231,7 +2248,7 @@
       <c r="D26" t="s">
         <v>99</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <v>1</v>
       </c>
       <c r="F26" t="s">
@@ -2240,7 +2257,7 @@
       <c r="G26" t="s">
         <v>15</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="2">
         <v>2</v>
       </c>
       <c r="I26" t="s">
@@ -2258,12 +2275,12 @@
       <c r="M26" t="s">
         <v>34</v>
       </c>
-      <c r="N26" t="b">
+      <c r="N26" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="2">
         <v>25</v>
       </c>
       <c r="B27" t="s">
@@ -2272,7 +2289,7 @@
       <c r="D27" t="s">
         <v>74</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <v>1</v>
       </c>
       <c r="F27" t="s">
@@ -2281,7 +2298,7 @@
       <c r="G27" t="s">
         <v>15</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="2">
         <v>6</v>
       </c>
       <c r="I27" t="s">
@@ -2299,12 +2316,12 @@
       <c r="M27" t="s">
         <v>29</v>
       </c>
-      <c r="N27" t="b">
+      <c r="N27" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="A28" s="2">
         <v>26</v>
       </c>
       <c r="B28" t="s">
@@ -2313,7 +2330,7 @@
       <c r="D28" t="s">
         <v>76</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="2">
         <v>1</v>
       </c>
       <c r="F28" t="s">
@@ -2322,7 +2339,7 @@
       <c r="G28" t="s">
         <v>15</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="2">
         <v>10</v>
       </c>
       <c r="I28" t="s">
@@ -2340,12 +2357,12 @@
       <c r="M28" t="s">
         <v>29</v>
       </c>
-      <c r="N28" t="b">
+      <c r="N28" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="A29" s="2">
         <v>27</v>
       </c>
       <c r="B29" t="s">
@@ -2354,7 +2371,7 @@
       <c r="D29" t="s">
         <v>78</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="2">
         <v>1</v>
       </c>
       <c r="F29" t="s">
@@ -2363,7 +2380,7 @@
       <c r="G29" t="s">
         <v>15</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="2">
         <v>8</v>
       </c>
       <c r="I29" t="s">
@@ -2381,12 +2398,12 @@
       <c r="M29" t="s">
         <v>100</v>
       </c>
-      <c r="N29" t="b">
+      <c r="N29" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="A30" s="2">
         <v>28</v>
       </c>
       <c r="B30" t="s">
@@ -2395,7 +2412,7 @@
       <c r="D30" t="s">
         <v>80</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="2">
         <v>1</v>
       </c>
       <c r="F30" t="s">
@@ -2404,7 +2421,7 @@
       <c r="G30" t="s">
         <v>15</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="2">
         <v>10</v>
       </c>
       <c r="I30" t="s">
@@ -2422,12 +2439,12 @@
       <c r="M30" t="s">
         <v>29</v>
       </c>
-      <c r="N30" t="b">
+      <c r="N30" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="2">
         <v>29</v>
       </c>
       <c r="B31" t="s">
@@ -2439,7 +2456,7 @@
       <c r="D31" t="s">
         <v>90</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="2">
         <v>1</v>
       </c>
       <c r="F31" t="s">
@@ -2448,7 +2465,7 @@
       <c r="G31" t="s">
         <v>15</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="2">
         <v>2</v>
       </c>
       <c r="I31" t="s">
@@ -2466,12 +2483,12 @@
       <c r="M31" t="s">
         <v>20</v>
       </c>
-      <c r="N31" t="b">
+      <c r="N31" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="A32" s="2">
         <v>30</v>
       </c>
       <c r="B32" t="s">
@@ -2483,7 +2500,7 @@
       <c r="D32" t="s">
         <v>90</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="2">
         <v>1</v>
       </c>
       <c r="F32" t="s">
@@ -2492,7 +2509,7 @@
       <c r="G32" t="s">
         <v>15</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="2">
         <v>2</v>
       </c>
       <c r="I32" t="s">
@@ -2510,12 +2527,12 @@
       <c r="M32" t="s">
         <v>20</v>
       </c>
-      <c r="N32" t="b">
+      <c r="N32" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="A33" s="2">
         <v>31</v>
       </c>
       <c r="B33" t="s">
@@ -2527,7 +2544,7 @@
       <c r="D33" t="s">
         <v>91</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="2">
         <v>1</v>
       </c>
       <c r="F33" t="s">
@@ -2536,7 +2553,7 @@
       <c r="G33" t="s">
         <v>15</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="2">
         <v>2</v>
       </c>
       <c r="I33" t="s">
@@ -2554,12 +2571,12 @@
       <c r="M33" t="s">
         <v>20</v>
       </c>
-      <c r="N33" t="b">
+      <c r="N33" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="A34" s="2">
         <v>32</v>
       </c>
       <c r="B34" t="s">
@@ -2568,7 +2585,7 @@
       <c r="D34" t="s">
         <v>86</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="2">
         <v>1</v>
       </c>
       <c r="F34" t="s">
@@ -2577,7 +2594,7 @@
       <c r="G34" t="s">
         <v>15</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="2">
         <v>5</v>
       </c>
       <c r="I34" t="s">
@@ -2595,12 +2612,12 @@
       <c r="M34" t="s">
         <v>29</v>
       </c>
-      <c r="N34" t="b">
+      <c r="N34" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A35">
+      <c r="A35" s="2">
         <v>33</v>
       </c>
       <c r="B35" t="s">
@@ -2612,7 +2629,7 @@
       <c r="D35" t="s">
         <v>89</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="2">
         <v>1</v>
       </c>
       <c r="F35" s="1" t="s">
@@ -2621,7 +2638,7 @@
       <c r="G35" t="s">
         <v>15</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="2">
         <v>4</v>
       </c>
       <c r="I35" t="s">
@@ -2639,12 +2656,12 @@
       <c r="M35" t="s">
         <v>20</v>
       </c>
-      <c r="N35" t="b">
+      <c r="N35" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="A36" s="2">
         <v>34</v>
       </c>
       <c r="B36" t="s">
@@ -2656,7 +2673,7 @@
       <c r="D36" t="s">
         <v>106</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="2">
         <v>1</v>
       </c>
       <c r="F36" s="1" t="s">
@@ -2665,7 +2682,7 @@
       <c r="G36" t="s">
         <v>15</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="2">
         <v>4</v>
       </c>
       <c r="I36" t="s">
@@ -2683,12 +2700,12 @@
       <c r="M36" t="s">
         <v>107</v>
       </c>
-      <c r="N36" t="b">
+      <c r="N36" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A37">
+      <c r="A37" s="2">
         <v>35</v>
       </c>
       <c r="B37" t="s">
@@ -2700,7 +2717,7 @@
       <c r="D37" t="s">
         <v>124</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="2">
         <v>1</v>
       </c>
       <c r="F37" s="1" t="s">
@@ -2709,7 +2726,7 @@
       <c r="G37" t="s">
         <v>15</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="2">
         <v>4</v>
       </c>
       <c r="I37" t="s">
@@ -2727,12 +2744,12 @@
       <c r="M37" t="s">
         <v>110</v>
       </c>
-      <c r="N37" t="b">
+      <c r="N37" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="A38" s="2">
         <v>36</v>
       </c>
       <c r="B38" t="s">
@@ -2744,7 +2761,7 @@
       <c r="D38" t="s">
         <v>113</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>1</v>
       </c>
       <c r="F38" s="1" t="s">
@@ -2753,7 +2770,7 @@
       <c r="G38" t="s">
         <v>15</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="2">
         <v>4</v>
       </c>
       <c r="I38" t="s">
@@ -2771,12 +2788,12 @@
       <c r="M38" t="s">
         <v>107</v>
       </c>
-      <c r="N38" t="b">
+      <c r="N38" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="A39" s="2">
         <v>37</v>
       </c>
       <c r="B39" t="s">
@@ -2788,7 +2805,7 @@
       <c r="D39" t="s">
         <v>117</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="2">
         <v>1</v>
       </c>
       <c r="F39" s="1" t="s">
@@ -2797,7 +2814,7 @@
       <c r="G39" t="s">
         <v>15</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="2">
         <v>5</v>
       </c>
       <c r="I39" t="s">
@@ -2815,12 +2832,12 @@
       <c r="M39" t="s">
         <v>118</v>
       </c>
-      <c r="N39" t="b">
+      <c r="N39" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="A40" s="2">
         <v>38</v>
       </c>
       <c r="B40" t="s">
@@ -2829,7 +2846,7 @@
       <c r="D40" t="s">
         <v>120</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="2">
         <v>1</v>
       </c>
       <c r="F40" s="1" t="s">
@@ -2838,7 +2855,7 @@
       <c r="G40" t="s">
         <v>15</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="2">
         <v>5</v>
       </c>
       <c r="I40" t="s">
@@ -2856,12 +2873,12 @@
       <c r="M40" t="s">
         <v>102</v>
       </c>
-      <c r="N40" t="b">
+      <c r="N40" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41">
+      <c r="A41" s="2">
         <v>39</v>
       </c>
       <c r="B41" t="s">
@@ -2870,7 +2887,7 @@
       <c r="D41" t="s">
         <v>122</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="2">
         <v>1</v>
       </c>
       <c r="F41" s="1" t="s">
@@ -2879,7 +2896,7 @@
       <c r="G41" t="s">
         <v>15</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="2">
         <v>2</v>
       </c>
       <c r="I41" t="s">
@@ -2897,12 +2914,12 @@
       <c r="M41" t="s">
         <v>102</v>
       </c>
-      <c r="N41" t="b">
+      <c r="N41" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A42">
+      <c r="A42" s="2">
         <v>40</v>
       </c>
       <c r="B42" t="s">
@@ -2914,7 +2931,7 @@
       <c r="D42" t="s">
         <v>127</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="2">
         <v>1</v>
       </c>
       <c r="F42" s="1" t="s">
@@ -2923,7 +2940,7 @@
       <c r="G42" t="s">
         <v>128</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="2">
         <v>15</v>
       </c>
       <c r="I42" t="s">
@@ -2941,12 +2958,12 @@
       <c r="M42" t="s">
         <v>102</v>
       </c>
-      <c r="N42" t="b">
+      <c r="N42" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A43">
+      <c r="A43" s="2">
         <v>41</v>
       </c>
       <c r="B43" t="s">
@@ -2958,7 +2975,7 @@
       <c r="D43" t="s">
         <v>132</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="2">
         <v>1</v>
       </c>
       <c r="F43" s="1" t="s">
@@ -2967,7 +2984,7 @@
       <c r="G43" t="s">
         <v>133</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="2">
         <v>2</v>
       </c>
       <c r="I43" t="s">
@@ -2985,12 +3002,12 @@
       <c r="M43" t="s">
         <v>134</v>
       </c>
-      <c r="N43" t="b">
+      <c r="N43" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44">
+      <c r="A44" s="2">
         <v>42</v>
       </c>
       <c r="B44" t="s">
@@ -3002,7 +3019,7 @@
       <c r="D44" t="s">
         <v>137</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="2">
         <v>1</v>
       </c>
       <c r="F44" s="1" t="s">
@@ -3011,7 +3028,7 @@
       <c r="G44" t="s">
         <v>133</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="2">
         <v>5</v>
       </c>
       <c r="I44" t="s">
@@ -3029,12 +3046,12 @@
       <c r="M44" t="s">
         <v>102</v>
       </c>
-      <c r="N44" t="b">
+      <c r="N44" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45">
+      <c r="A45" s="2">
         <v>43</v>
       </c>
       <c r="B45" t="s">
@@ -3046,7 +3063,7 @@
       <c r="D45" t="s">
         <v>140</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="2">
         <v>3</v>
       </c>
       <c r="F45" s="1" t="s">
@@ -3055,7 +3072,7 @@
       <c r="G45" t="s">
         <v>133</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="2">
         <v>4</v>
       </c>
       <c r="I45" t="s">
@@ -3073,12 +3090,12 @@
       <c r="M45" t="s">
         <v>141</v>
       </c>
-      <c r="N45" t="b">
+      <c r="N45" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A46">
+      <c r="A46" s="2">
         <v>44</v>
       </c>
       <c r="B46" t="s">
@@ -3090,7 +3107,7 @@
       <c r="D46" t="s">
         <v>144</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="2">
         <v>1</v>
       </c>
       <c r="F46" s="1" t="s">
@@ -3099,7 +3116,7 @@
       <c r="G46" t="s">
         <v>133</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="2">
         <v>15</v>
       </c>
       <c r="I46" t="s">
@@ -3117,12 +3134,12 @@
       <c r="M46" t="s">
         <v>102</v>
       </c>
-      <c r="N46" t="b">
+      <c r="N46" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A47">
+      <c r="A47" s="2">
         <v>45</v>
       </c>
       <c r="B47" t="s">
@@ -3134,7 +3151,7 @@
       <c r="D47" t="s">
         <v>148</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="2">
         <v>1</v>
       </c>
       <c r="F47" s="1" t="s">
@@ -3143,7 +3160,7 @@
       <c r="G47" t="s">
         <v>133</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="2">
         <v>0</v>
       </c>
       <c r="I47" t="s">
@@ -3161,12 +3178,12 @@
       <c r="M47" t="s">
         <v>150</v>
       </c>
-      <c r="N47" t="b">
+      <c r="N47" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48">
+      <c r="A48" s="2">
         <v>46</v>
       </c>
       <c r="B48" t="s">
@@ -3178,7 +3195,7 @@
       <c r="D48" t="s">
         <v>153</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="2">
         <v>1</v>
       </c>
       <c r="F48" s="1" t="s">
@@ -3187,7 +3204,7 @@
       <c r="G48" t="s">
         <v>133</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="2">
         <v>7</v>
       </c>
       <c r="I48" t="s">
@@ -3205,12 +3222,12 @@
       <c r="M48" t="s">
         <v>102</v>
       </c>
-      <c r="N48" t="b">
+      <c r="N48" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A49">
+      <c r="A49" s="2">
         <v>47</v>
       </c>
       <c r="B49" t="s">
@@ -3222,7 +3239,7 @@
       <c r="D49" t="s">
         <v>156</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="2">
         <v>1</v>
       </c>
       <c r="F49" s="1" t="s">
@@ -3231,7 +3248,7 @@
       <c r="G49" t="s">
         <v>133</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="2">
         <v>6</v>
       </c>
       <c r="I49" t="s">
@@ -3249,12 +3266,12 @@
       <c r="M49" t="s">
         <v>102</v>
       </c>
-      <c r="N49" t="b">
+      <c r="N49" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A50">
+      <c r="A50" s="2">
         <v>48</v>
       </c>
       <c r="B50" t="s">
@@ -3266,7 +3283,7 @@
       <c r="D50" t="s">
         <v>160</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="2">
         <v>1</v>
       </c>
       <c r="F50" s="1" t="s">
@@ -3275,7 +3292,7 @@
       <c r="G50" t="s">
         <v>133</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="2">
         <v>7</v>
       </c>
       <c r="I50" t="s">
@@ -3293,12 +3310,12 @@
       <c r="M50" t="s">
         <v>161</v>
       </c>
-      <c r="N50" t="b">
+      <c r="N50" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A51">
+      <c r="A51" s="2">
         <v>49</v>
       </c>
       <c r="B51" t="s">
@@ -3310,7 +3327,7 @@
       <c r="D51" t="s">
         <v>164</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="2">
         <v>1</v>
       </c>
       <c r="F51" s="1" t="s">
@@ -3319,7 +3336,7 @@
       <c r="G51" t="s">
         <v>133</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="2">
         <v>7</v>
       </c>
       <c r="I51" t="s">
@@ -3337,12 +3354,12 @@
       <c r="M51" t="s">
         <v>165</v>
       </c>
-      <c r="N51" t="b">
+      <c r="N51" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A52">
+      <c r="A52" s="2">
         <v>50</v>
       </c>
       <c r="B52" t="s">
@@ -3354,7 +3371,7 @@
       <c r="D52" t="s">
         <v>168</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="2">
         <v>1</v>
       </c>
       <c r="F52" s="1" t="s">
@@ -3363,7 +3380,7 @@
       <c r="G52" t="s">
         <v>133</v>
       </c>
-      <c r="H52">
+      <c r="H52" s="2">
         <v>5</v>
       </c>
       <c r="I52" t="s">
@@ -3381,12 +3398,12 @@
       <c r="M52" t="s">
         <v>102</v>
       </c>
-      <c r="N52" t="b">
+      <c r="N52" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A53">
+      <c r="A53" s="2">
         <v>51</v>
       </c>
       <c r="B53" t="s">
@@ -3398,7 +3415,7 @@
       <c r="D53" t="s">
         <v>174</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="2">
         <v>3</v>
       </c>
       <c r="F53" s="1" t="s">
@@ -3407,7 +3424,7 @@
       <c r="G53" t="s">
         <v>133</v>
       </c>
-      <c r="H53">
+      <c r="H53" s="2">
         <v>-1</v>
       </c>
       <c r="I53" t="s">
@@ -3425,12 +3442,12 @@
       <c r="M53" t="s">
         <v>178</v>
       </c>
-      <c r="N53" t="b">
+      <c r="N53" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A54">
+      <c r="A54" s="2">
         <v>52</v>
       </c>
       <c r="B54" t="s">
@@ -3442,7 +3459,7 @@
       <c r="D54" t="s">
         <v>181</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="2">
         <v>3</v>
       </c>
       <c r="F54" s="1" t="s">
@@ -3451,7 +3468,7 @@
       <c r="G54" t="s">
         <v>133</v>
       </c>
-      <c r="H54">
+      <c r="H54" s="2">
         <v>-1</v>
       </c>
       <c r="I54" t="s">
@@ -3469,12 +3486,12 @@
       <c r="M54" t="s">
         <v>182</v>
       </c>
-      <c r="N54" t="b">
+      <c r="N54" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A55">
+      <c r="A55" s="2">
         <v>53</v>
       </c>
       <c r="B55" t="s">
@@ -3486,7 +3503,7 @@
       <c r="D55" t="s">
         <v>185</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="2">
         <v>3</v>
       </c>
       <c r="F55" s="1" t="s">
@@ -3495,7 +3512,7 @@
       <c r="G55" t="s">
         <v>133</v>
       </c>
-      <c r="H55">
+      <c r="H55" s="2">
         <v>-1</v>
       </c>
       <c r="I55" t="s">
@@ -3513,12 +3530,12 @@
       <c r="M55" t="s">
         <v>187</v>
       </c>
-      <c r="N55" t="b">
+      <c r="N55" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A56">
+      <c r="A56" s="2">
         <v>54</v>
       </c>
       <c r="B56" t="s">
@@ -3530,7 +3547,7 @@
       <c r="D56" t="s">
         <v>190</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="2">
         <v>3</v>
       </c>
       <c r="F56" s="1" t="s">
@@ -3539,7 +3556,7 @@
       <c r="G56" t="s">
         <v>133</v>
       </c>
-      <c r="H56">
+      <c r="H56" s="2">
         <v>-1</v>
       </c>
       <c r="I56" t="s">
@@ -3557,12 +3574,12 @@
       <c r="M56" t="s">
         <v>192</v>
       </c>
-      <c r="N56" t="b">
+      <c r="N56" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A57">
+      <c r="A57" s="2">
         <v>55</v>
       </c>
       <c r="B57" t="s">
@@ -3574,7 +3591,7 @@
       <c r="D57" t="s">
         <v>195</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="2">
         <v>3</v>
       </c>
       <c r="F57" s="1" t="s">
@@ -3583,7 +3600,7 @@
       <c r="G57" t="s">
         <v>133</v>
       </c>
-      <c r="H57">
+      <c r="H57" s="2">
         <v>-1</v>
       </c>
       <c r="I57" t="s">
@@ -3601,12 +3618,12 @@
       <c r="M57" t="s">
         <v>197</v>
       </c>
-      <c r="N57" t="b">
+      <c r="N57" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A58">
+      <c r="A58" s="2">
         <v>56</v>
       </c>
       <c r="B58" t="s">
@@ -3618,7 +3635,7 @@
       <c r="D58" t="s">
         <v>200</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="2">
         <v>3</v>
       </c>
       <c r="F58" s="1" t="s">
@@ -3627,7 +3644,7 @@
       <c r="G58" t="s">
         <v>133</v>
       </c>
-      <c r="H58">
+      <c r="H58" s="2">
         <v>0</v>
       </c>
       <c r="I58" t="s">
@@ -3645,12 +3662,12 @@
       <c r="M58" t="s">
         <v>202</v>
       </c>
-      <c r="N58" t="b">
+      <c r="N58" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A59">
+      <c r="A59" s="2">
         <v>57</v>
       </c>
       <c r="B59" t="s">
@@ -3662,7 +3679,7 @@
       <c r="D59" t="s">
         <v>205</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="2">
         <v>3</v>
       </c>
       <c r="F59" s="1" t="s">
@@ -3671,7 +3688,7 @@
       <c r="G59" t="s">
         <v>133</v>
       </c>
-      <c r="H59">
+      <c r="H59" s="2">
         <v>-1</v>
       </c>
       <c r="I59" t="s">
@@ -3689,644 +3706,644 @@
       <c r="M59" t="s">
         <v>207</v>
       </c>
-      <c r="N59" t="b">
+      <c r="N59" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A60">
+      <c r="A60" s="2">
         <v>58</v>
       </c>
       <c r="F60" s="1"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A61">
+      <c r="A61" s="2">
         <v>59</v>
       </c>
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A62">
+      <c r="A62" s="2">
         <v>60</v>
       </c>
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A63">
+      <c r="A63" s="2">
         <v>61</v>
       </c>
       <c r="F63" s="1"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A64">
+      <c r="A64" s="2">
         <v>62</v>
       </c>
       <c r="F64" s="1"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65">
+      <c r="A65" s="2">
         <v>63</v>
       </c>
       <c r="F65" s="1"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66">
+      <c r="A66" s="2">
         <v>64</v>
       </c>
       <c r="F66" s="1"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67">
+      <c r="A67" s="2">
         <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68">
+      <c r="A68" s="2">
         <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69">
+      <c r="A69" s="2">
         <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70">
+      <c r="A70" s="2">
         <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71">
+      <c r="A71" s="2">
         <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72">
+      <c r="A72" s="2">
         <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73">
+      <c r="A73" s="2">
         <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74">
+      <c r="A74" s="2">
         <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75">
+      <c r="A75" s="2">
         <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76">
+      <c r="A76" s="2">
         <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77">
+      <c r="A77" s="2">
         <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78">
+      <c r="A78" s="2">
         <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79">
+      <c r="A79" s="2">
         <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80">
+      <c r="A80" s="2">
         <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81">
+      <c r="A81" s="2">
         <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82">
+      <c r="A82" s="2">
         <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83">
+      <c r="A83" s="2">
         <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84">
+      <c r="A84" s="2">
         <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85">
+      <c r="A85" s="2">
         <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86">
+      <c r="A86" s="2">
         <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87">
+      <c r="A87" s="2">
         <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88">
+      <c r="A88" s="2">
         <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A89">
+      <c r="A89" s="2">
         <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A90">
+      <c r="A90" s="2">
         <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A91">
+      <c r="A91" s="2">
         <v>89</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A92">
+      <c r="A92" s="2">
         <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A93">
+      <c r="A93" s="2">
         <v>91</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A94">
+      <c r="A94" s="2">
         <v>92</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A95">
+      <c r="A95" s="2">
         <v>93</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A96">
+      <c r="A96" s="2">
         <v>94</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97">
+      <c r="A97" s="2">
         <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A98">
+      <c r="A98" s="2">
         <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A99">
+      <c r="A99" s="2">
         <v>97</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100">
+      <c r="A100" s="2">
         <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101">
+      <c r="A101" s="2">
         <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A102">
+      <c r="A102" s="2">
         <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A103">
+      <c r="A103" s="2">
         <v>101</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A104">
+      <c r="A104" s="2">
         <v>102</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105">
+      <c r="A105" s="2">
         <v>103</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A106">
+      <c r="A106" s="2">
         <v>104</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107">
+      <c r="A107" s="2">
         <v>105</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A108">
+      <c r="A108" s="2">
         <v>106</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A109">
+      <c r="A109" s="2">
         <v>107</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A110">
+      <c r="A110" s="2">
         <v>108</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A111">
+      <c r="A111" s="2">
         <v>109</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A112">
+      <c r="A112" s="2">
         <v>110</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A113">
+      <c r="A113" s="2">
         <v>111</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A114">
+      <c r="A114" s="2">
         <v>112</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A115">
+      <c r="A115" s="2">
         <v>113</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A116">
+      <c r="A116" s="2">
         <v>114</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A117">
+      <c r="A117" s="2">
         <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A118">
+      <c r="A118" s="2">
         <v>116</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A119">
+      <c r="A119" s="2">
         <v>117</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A120">
+      <c r="A120" s="2">
         <v>118</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A121">
+      <c r="A121" s="2">
         <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A122">
+      <c r="A122" s="2">
         <v>120</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A123">
+      <c r="A123" s="2">
         <v>121</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A124">
+      <c r="A124" s="2">
         <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A125">
+      <c r="A125" s="2">
         <v>123</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A126">
+      <c r="A126" s="2">
         <v>124</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A127">
+      <c r="A127" s="2">
         <v>125</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A128">
+      <c r="A128" s="2">
         <v>126</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A129">
+      <c r="A129" s="2">
         <v>127</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A130">
+      <c r="A130" s="2">
         <v>128</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A131">
+      <c r="A131" s="2">
         <v>129</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A132">
+      <c r="A132" s="2">
         <v>130</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A133">
+      <c r="A133" s="2">
         <v>131</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A134">
+      <c r="A134" s="2">
         <v>132</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A135">
+      <c r="A135" s="2">
         <v>133</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A136">
+      <c r="A136" s="2">
         <v>134</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A137">
+      <c r="A137" s="2">
         <v>135</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A138">
+      <c r="A138" s="2">
         <v>136</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A139">
+      <c r="A139" s="2">
         <v>137</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A140">
+      <c r="A140" s="2">
         <v>138</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A141">
+      <c r="A141" s="2">
         <v>139</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A142">
+      <c r="A142" s="2">
         <v>140</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A143">
+      <c r="A143" s="2">
         <v>141</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A144">
+      <c r="A144" s="2">
         <v>142</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A145">
+      <c r="A145" s="2">
         <v>143</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A146">
+      <c r="A146" s="2">
         <v>144</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A147">
+      <c r="A147" s="2">
         <v>145</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A148">
+      <c r="A148" s="2">
         <v>146</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A149">
+      <c r="A149" s="2">
         <v>147</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A150">
+      <c r="A150" s="2">
         <v>148</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A151">
+      <c r="A151" s="2">
         <v>149</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A152">
+      <c r="A152" s="2">
         <v>150</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A153">
+      <c r="A153" s="2">
         <v>151</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A154">
+      <c r="A154" s="2">
         <v>152</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A155">
+      <c r="A155" s="2">
         <v>153</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A156">
+      <c r="A156" s="2">
         <v>154</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A157">
+      <c r="A157" s="2">
         <v>155</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A158">
+      <c r="A158" s="2">
         <v>156</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A159">
+      <c r="A159" s="2">
         <v>157</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A160">
+      <c r="A160" s="2">
         <v>158</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A161">
+      <c r="A161" s="2">
         <v>159</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A162">
+      <c r="A162" s="2">
         <v>160</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A163">
+      <c r="A163" s="2">
         <v>161</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A164">
+      <c r="A164" s="2">
         <v>162</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A165">
+      <c r="A165" s="2">
         <v>163</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A166">
+      <c r="A166" s="2">
         <v>164</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A167">
+      <c r="A167" s="2">
         <v>165</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A168">
+      <c r="A168" s="2">
         <v>166</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A169">
+      <c r="A169" s="2">
         <v>167</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A170">
+      <c r="A170" s="2">
         <v>168</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A171">
+      <c r="A171" s="2">
         <v>169</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A172">
+      <c r="A172" s="2">
         <v>170</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A173">
+      <c r="A173" s="2">
         <v>171</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A174">
+      <c r="A174" s="2">
         <v>172</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A175">
+      <c r="A175" s="2">
         <v>173</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A176">
+      <c r="A176" s="2">
         <v>174</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A177">
+      <c r="A177" s="2">
         <v>175</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A178">
+      <c r="A178" s="2">
         <v>176</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A179">
+      <c r="A179" s="2">
         <v>177</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A180">
+      <c r="A180" s="2">
         <v>178</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A181">
+      <c r="A181" s="2">
         <v>179</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A182">
+      <c r="A182" s="2">
         <v>180</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A183">
+      <c r="A183" s="2">
         <v>181</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A184">
+      <c r="A184" s="2">
         <v>182</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A185">
+      <c r="A185" s="2">
         <v>183</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Complete CardPoolDatabase before id=57
</commit_message>
<xml_diff>
--- a/Resources/CardPoolDatabase.xlsx
+++ b/Resources/CardPoolDatabase.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cpp\GwentCore\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Junce\Source\Repos\GwentCore\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="225">
   <si>
     <t>Name</t>
   </si>
@@ -757,6 +757,60 @@
   </si>
   <si>
     <t>SpellScorch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Endrega.png</t>
+  </si>
+  <si>
+    <t>Fiend.png</t>
+  </si>
+  <si>
+    <t>Fire Elemental.png</t>
+  </si>
+  <si>
+    <t>Foglet.png</t>
+  </si>
+  <si>
+    <t>Forktail.png</t>
+  </si>
+  <si>
+    <t>Frightener.png</t>
+  </si>
+  <si>
+    <t>Gargoyle.png</t>
+  </si>
+  <si>
+    <t>Grave Hag.png</t>
+  </si>
+  <si>
+    <t>Griffin.png</t>
+  </si>
+  <si>
+    <t>Harpy.png</t>
+  </si>
+  <si>
+    <t>Ice Giant.png</t>
+  </si>
+  <si>
+    <t>Imlerith.png</t>
+  </si>
+  <si>
+    <t>Kayran.png</t>
+  </si>
+  <si>
+    <t>Leshen.png</t>
+  </si>
+  <si>
+    <t>Plague Maiden.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Werewolf.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wyvern.png</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1141,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q185"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1154,7 +1208,7 @@
     <col min="5" max="5" width="2.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="6.625" customWidth="1"/>
     <col min="7" max="7" width="4.625" customWidth="1"/>
-    <col min="8" max="8" width="3.375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="4.375" style="2" customWidth="1"/>
     <col min="9" max="9" width="9.375" customWidth="1"/>
     <col min="10" max="10" width="7.625" customWidth="1"/>
     <col min="11" max="11" width="5.375" customWidth="1"/>
@@ -1339,7 +1393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1744,6 +1798,9 @@
       <c r="B14" t="s">
         <v>54</v>
       </c>
+      <c r="C14" t="s">
+        <v>208</v>
+      </c>
       <c r="D14" t="s">
         <v>94</v>
       </c>
@@ -1785,6 +1842,9 @@
       <c r="B15" t="s">
         <v>55</v>
       </c>
+      <c r="C15" t="s">
+        <v>209</v>
+      </c>
       <c r="D15" t="s">
         <v>95</v>
       </c>
@@ -1825,6 +1885,9 @@
       </c>
       <c r="B16" t="s">
         <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>210</v>
       </c>
       <c r="D16" t="s">
         <v>57</v>
@@ -1867,6 +1930,9 @@
       <c r="B17" t="s">
         <v>58</v>
       </c>
+      <c r="C17" t="s">
+        <v>211</v>
+      </c>
       <c r="D17" t="s">
         <v>59</v>
       </c>
@@ -1908,6 +1974,9 @@
       <c r="B18" t="s">
         <v>60</v>
       </c>
+      <c r="C18" t="s">
+        <v>212</v>
+      </c>
       <c r="D18" t="s">
         <v>61</v>
       </c>
@@ -1949,6 +2018,9 @@
       <c r="B19" t="s">
         <v>62</v>
       </c>
+      <c r="C19" t="s">
+        <v>213</v>
+      </c>
       <c r="D19" t="s">
         <v>96</v>
       </c>
@@ -1989,6 +2061,9 @@
       </c>
       <c r="B20" t="s">
         <v>63</v>
+      </c>
+      <c r="C20" t="s">
+        <v>214</v>
       </c>
       <c r="D20" t="s">
         <v>97</v>
@@ -2163,6 +2238,9 @@
       <c r="B24" t="s">
         <v>69</v>
       </c>
+      <c r="C24" t="s">
+        <v>215</v>
+      </c>
       <c r="D24" t="s">
         <v>70</v>
       </c>
@@ -2204,6 +2282,9 @@
       <c r="B25" t="s">
         <v>71</v>
       </c>
+      <c r="C25" t="s">
+        <v>216</v>
+      </c>
       <c r="D25" t="s">
         <v>98</v>
       </c>
@@ -2245,6 +2326,9 @@
       <c r="B26" t="s">
         <v>72</v>
       </c>
+      <c r="C26" t="s">
+        <v>217</v>
+      </c>
       <c r="D26" t="s">
         <v>99</v>
       </c>
@@ -2286,6 +2370,9 @@
       <c r="B27" t="s">
         <v>73</v>
       </c>
+      <c r="C27" t="s">
+        <v>218</v>
+      </c>
       <c r="D27" t="s">
         <v>74</v>
       </c>
@@ -2327,6 +2414,9 @@
       <c r="B28" t="s">
         <v>75</v>
       </c>
+      <c r="C28" t="s">
+        <v>219</v>
+      </c>
       <c r="D28" t="s">
         <v>76</v>
       </c>
@@ -2368,6 +2458,9 @@
       <c r="B29" t="s">
         <v>77</v>
       </c>
+      <c r="C29" t="s">
+        <v>220</v>
+      </c>
       <c r="D29" t="s">
         <v>78</v>
       </c>
@@ -2409,6 +2502,9 @@
       <c r="B30" t="s">
         <v>79</v>
       </c>
+      <c r="C30" t="s">
+        <v>221</v>
+      </c>
       <c r="D30" t="s">
         <v>80</v>
       </c>
@@ -2582,6 +2678,9 @@
       <c r="B34" t="s">
         <v>85</v>
       </c>
+      <c r="C34" t="s">
+        <v>222</v>
+      </c>
       <c r="D34" t="s">
         <v>86</v>
       </c>
@@ -2843,6 +2942,9 @@
       <c r="B40" t="s">
         <v>119</v>
       </c>
+      <c r="C40" t="s">
+        <v>223</v>
+      </c>
       <c r="D40" t="s">
         <v>120</v>
       </c>
@@ -2883,6 +2985,9 @@
       </c>
       <c r="B41" t="s">
         <v>121</v>
+      </c>
+      <c r="C41" t="s">
+        <v>224</v>
       </c>
       <c r="D41" t="s">
         <v>122</v>

</xml_diff>

<commit_message>
have compeleted Card data base
</commit_message>
<xml_diff>
--- a/Resources/CardPoolDatabase.xlsx
+++ b/Resources/CardPoolDatabase.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="538">
   <si>
     <t>Name</t>
   </si>
@@ -1599,8 +1599,233 @@
     <t xml:space="preserve">Yarpen Zigrin.png </t>
   </si>
   <si>
-    <t>Defualt Meseage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>A fireball? Of course. Whatever Your Imperial Majesty wishes.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Niflgaardian mages do have a choice: servile submission, or the gallows.</t>
+  </si>
+  <si>
+    <t>I aim for the knee. Always.</t>
+  </si>
+  <si>
+    <t>His eyes flashed under his winged helmet. Fire gleamed from his sword's blade.</t>
+  </si>
+  <si>
+    <t>Cynthia's talents can be deadly. She needs a thight leash.</t>
+  </si>
+  <si>
+    <t>Double or nothing, aim for his cock.</t>
+  </si>
+  <si>
+    <t>Magic is the highest good. It transcends all borders and divisions.</t>
+  </si>
+  <si>
+    <t>Not the best for taking cities, but great for razing them to the ground.</t>
+  </si>
+  <si>
+    <t>The Impera Brigade never surrenders. Ever.</t>
+  </si>
+  <si>
+    <t>Witchers never die in their beds.</t>
+  </si>
+  <si>
+    <t>I'll take an attentive reconnaissance unit over a fine cavalry brigade any day.</t>
+  </si>
+  <si>
+    <t>No Nordling pikemen or dwarven spearbearers can hope to best trained cavalry.</t>
+  </si>
+  <si>
+    <t>Summer sun reflecting in the quiet waters of the Alba - that's Nilfgaard to me.</t>
+  </si>
+  <si>
+    <t>The Emperor will teach the North discipline.</t>
+  </si>
+  <si>
+    <t>Learned a lot at Braibant Military Academy. How to scrub potatoes, for instance.</t>
+  </si>
+  <si>
+    <t>You 'll die a painfully as that pathetic traitor Windhalm did.</t>
+  </si>
+  <si>
+    <t>They say the Impera fear nothing. Untrue. Renuald scares them shitless.</t>
+  </si>
+  <si>
+    <t>The rotten smell brings back childhood memories.</t>
+  </si>
+  <si>
+    <t>Warfare is mere sound and fury diplomacy is what truly shapes·history.</t>
+  </si>
+  <si>
+    <t>Wielded correctly, a protractor can be a deadly weapon.</t>
+  </si>
+  <si>
+    <t>I never miss twice.</t>
+  </si>
+  <si>
+    <t>My mark scars the face of our future empress. That is my proudest achievement.</t>
+  </si>
+  <si>
+    <t>And hands off the girl! Whatever we may be, we're not savages.</t>
+  </si>
+  <si>
+    <t>Albaaaa! Forward!! Alba! Long live the Emperor!</t>
+  </si>
+  <si>
+    <t>For a fire mage , he's not very ... flamboyant.</t>
+  </si>
+  <si>
+    <t>There's never been a problem a well-planned assassination couldn't solve.</t>
+  </si>
+  <si>
+    <t>Discipline is the Empire's deadliest weapon.</t>
+  </si>
+  <si>
+    <t>If I acquit myself well, perhaps next they' ll post me somewhere civilized.</t>
+  </si>
+  <si>
+    <t>The Zerrikanian Desert used to be a lush garden. Then these came along.</t>
+  </si>
+  <si>
+    <t>Usually we give 'em female nanes. -Like Jenny? -More like Bertha.</t>
+  </si>
+  <si>
+    <t>I'd anyhing for Temeria. Mostly, though, 1 kill for her.</t>
+  </si>
+  <si>
+    <t>The gods help those who have better catapults.</t>
+  </si>
+  <si>
+    <t>Haven't had much luck with monsters of late, -so we enlisted.</t>
+  </si>
+  <si>
+    <t>I once made a prisoner vomit his own entrails. . . Ah, good times. . .</t>
+  </si>
+  <si>
+    <t>Stitch red to red, white to white, and everything will be all right.</t>
+  </si>
+  <si>
+    <t>Like all Thyssen men, he was tall, powerfully built and criminally handsome.</t>
+  </si>
+  <si>
+    <t>Thlat square should bear the names of my soldiers, of the dead. Not mine.</t>
+  </si>
+  <si>
+    <t>You gota recalihrate the arm hy five degrees. - Do what by the what now?</t>
+  </si>
+  <si>
+    <t>If I'm to die today, I wish to look smashing for the occasion.</t>
+  </si>
+  <si>
+    <t>Soon the power of kings will wither，and the Lodge shall seize its rightful place.</t>
+  </si>
+  <si>
+    <t>I's a war veteran! ... spare me a crown?</t>
+  </si>
+  <si>
+    <t>He ploughin' wears golden armor. Golden. Course he's an arsehole.</t>
+  </si>
+  <si>
+    <t>I've bled for Redania! I've killed for Redania. .. Dammit, I've even raped for Redania!</t>
+  </si>
+  <si>
+    <t>The Daughter of the Kaedweni Wilderness.</t>
+  </si>
+  <si>
+    <t>I was there， on the front lines! Right where the fightin' was the thickest!</t>
+  </si>
+  <si>
+    <t>I love the clamor of siege towers in the morning. Sounds like victory.</t>
+  </si>
+  <si>
+    <t>We're on the same side, witcher. You'll realize this one day.</t>
+  </si>
+  <si>
+    <t>Gwent's like politics, just more honest.</t>
+  </si>
+  <si>
+    <t>The Lodge lacks humility: Our lust for power may yet be our undoing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuck off! We aren't all ploughin'philanderers. Some of us have depth. . . </t>
+  </si>
+  <si>
+    <t>Castle won't batter itself down, now will it? Get them trebuchets rollin'!</t>
+  </si>
+  <si>
+    <t>A patriot... and a real son of a bitch.</t>
+  </si>
+  <si>
+    <t>Better to live one day as a king than a whole life as a beggar.</t>
+  </si>
+  <si>
+    <t>The world belongs to whoever's best at crackin' skulls and impregnatin' lasses.</t>
+  </si>
+  <si>
+    <t>Our mead smells like piss, do it? Easy to fix - I'll break your fuckin' nose!</t>
+  </si>
+  <si>
+    <t>The path to freedom is paved in blood, not ink.</t>
+  </si>
+  <si>
+    <t>I know how to carry out orders, so you can shove you advice up your coal chute.</t>
+  </si>
+  <si>
+    <t>Take another step, dh'oine. You a look better with an arrow between your eyes.</t>
+  </si>
+  <si>
+    <t>They track like hounds, run like deer and kill like cold -hearted bastards.</t>
+  </si>
+  <si>
+    <t>Worked a pickaxe all me life. Battleaxe won't be any trouble.</t>
+  </si>
+  <si>
+    <t>The dryad queen has eyes of molten silver, and a heart of cold -forged steel.</t>
+  </si>
+  <si>
+    <t>No matter what you may have heard, elves don't take human scalps. Too much lice.</t>
+  </si>
+  <si>
+    <t>Though we are now few and scattered, our hearts burn brighter than ever.</t>
+  </si>
+  <si>
+    <t>Sure, I'll patch you up. Gonna cost you, though.</t>
+  </si>
+  <si>
+    <t>I fight for whoever's paying the best. Or whoever's easiest to rob.</t>
+  </si>
+  <si>
+    <t>I am a Sage. My power lies in possessing knowledge. Not sharing it.</t>
+  </si>
+  <si>
+    <t>King or beggar, what's the difference? One dh'oine less.</t>
+  </si>
+  <si>
+    <t>It dawns on them once they notice my scar: a realization of imminent death.</t>
+  </si>
+  <si>
+    <t>I'm telling ye, we're born fer battle - we slash straight at their knees!</t>
+  </si>
+  <si>
+    <t>With each arrow I loose, I think of my da. Heli be proud. I think.</t>
+  </si>
+  <si>
+    <t>Stare into their eyes , feast on their terror. Then go in for the kill.</t>
+  </si>
+  <si>
+    <t>Beautiful, pure, fierce - the perfect icon for a rebellion.</t>
+  </si>
+  <si>
+    <t>Time to look death in the face.</t>
+  </si>
+  <si>
+    <t>I'd gladly kill you from up close, stare in your eyes ... But you reek, human.</t>
+  </si>
+  <si>
+    <t>Vrihedd? What's that mean? - Trouble.</t>
+  </si>
+  <si>
+    <t>We are the drops of rain that together make a ferocious storm.</t>
   </si>
 </sst>
 </file>
@@ -1993,8 +2218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M173" sqref="M173"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D153" sqref="D153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2003,8 +2228,8 @@
     <col min="2" max="2" width="13.375" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="34.125" customWidth="1"/>
-    <col min="5" max="5" width="23.125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="5.25" customWidth="1"/>
+    <col min="5" max="5" width="8.125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.625" customWidth="1"/>
     <col min="7" max="7" width="8.375" customWidth="1"/>
     <col min="8" max="8" width="4.375" style="2" customWidth="1"/>
     <col min="9" max="9" width="14.125" customWidth="1"/>
@@ -4709,7 +4934,7 @@
         <v>388</v>
       </c>
       <c r="D62" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="E62" s="7">
         <v>1</v>
@@ -4753,7 +4978,7 @@
         <v>389</v>
       </c>
       <c r="D63" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E63" s="7">
         <v>1</v>
@@ -4797,7 +5022,7 @@
         <v>390</v>
       </c>
       <c r="D64" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E64" s="7">
         <v>1</v>
@@ -4841,7 +5066,7 @@
         <v>391</v>
       </c>
       <c r="D65" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="E65" s="7">
         <v>1</v>
@@ -4885,7 +5110,7 @@
         <v>392</v>
       </c>
       <c r="D66" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="E66" s="7">
         <v>1</v>
@@ -4929,7 +5154,7 @@
         <v>393</v>
       </c>
       <c r="D67" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="E67" s="7">
         <v>1</v>
@@ -4973,7 +5198,7 @@
         <v>394</v>
       </c>
       <c r="D68" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="E68" s="7">
         <v>1</v>
@@ -5017,7 +5242,7 @@
         <v>395</v>
       </c>
       <c r="D69" t="s">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="E69" s="7">
         <v>1</v>
@@ -5061,7 +5286,7 @@
         <v>396</v>
       </c>
       <c r="D70" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="E70" s="7">
         <v>1</v>
@@ -5105,7 +5330,7 @@
         <v>397</v>
       </c>
       <c r="D71" t="s">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="E71" s="7">
         <v>1</v>
@@ -5149,7 +5374,7 @@
         <v>398</v>
       </c>
       <c r="D72" t="s">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="E72" s="7">
         <v>1</v>
@@ -5193,7 +5418,7 @@
         <v>399</v>
       </c>
       <c r="D73" t="s">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="E73" s="7">
         <v>1</v>
@@ -5237,7 +5462,7 @@
         <v>400</v>
       </c>
       <c r="D74" t="s">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="E74" s="7">
         <v>1</v>
@@ -5281,7 +5506,7 @@
         <v>401</v>
       </c>
       <c r="D75" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
       <c r="E75" s="7">
         <v>1</v>
@@ -5325,7 +5550,7 @@
         <v>402</v>
       </c>
       <c r="D76" t="s">
-        <v>462</v>
+        <v>472</v>
       </c>
       <c r="E76" s="7">
         <v>1</v>
@@ -5369,7 +5594,7 @@
         <v>403</v>
       </c>
       <c r="D77" t="s">
-        <v>462</v>
+        <v>473</v>
       </c>
       <c r="E77" s="7">
         <v>1</v>
@@ -5413,7 +5638,7 @@
         <v>404</v>
       </c>
       <c r="D78" t="s">
-        <v>462</v>
+        <v>474</v>
       </c>
       <c r="E78" s="7">
         <v>1</v>
@@ -5457,7 +5682,7 @@
         <v>405</v>
       </c>
       <c r="D79" t="s">
-        <v>462</v>
+        <v>475</v>
       </c>
       <c r="E79" s="7">
         <v>1</v>
@@ -5501,7 +5726,7 @@
         <v>406</v>
       </c>
       <c r="D80" t="s">
-        <v>462</v>
+        <v>475</v>
       </c>
       <c r="E80" s="7">
         <v>1</v>
@@ -5545,7 +5770,7 @@
         <v>407</v>
       </c>
       <c r="D81" t="s">
-        <v>462</v>
+        <v>475</v>
       </c>
       <c r="E81" s="7">
         <v>1</v>
@@ -5589,7 +5814,7 @@
         <v>408</v>
       </c>
       <c r="D82" t="s">
-        <v>462</v>
+        <v>476</v>
       </c>
       <c r="E82" s="7">
         <v>1</v>
@@ -5633,7 +5858,7 @@
         <v>409</v>
       </c>
       <c r="D83" t="s">
-        <v>462</v>
+        <v>477</v>
       </c>
       <c r="E83" s="7">
         <v>1</v>
@@ -5677,7 +5902,7 @@
         <v>410</v>
       </c>
       <c r="D84" t="s">
-        <v>462</v>
+        <v>478</v>
       </c>
       <c r="E84" s="7">
         <v>1</v>
@@ -5721,7 +5946,7 @@
         <v>411</v>
       </c>
       <c r="D85" t="s">
-        <v>462</v>
+        <v>479</v>
       </c>
       <c r="E85" s="7">
         <v>1</v>
@@ -5765,7 +5990,7 @@
         <v>412</v>
       </c>
       <c r="D86" t="s">
-        <v>462</v>
+        <v>480</v>
       </c>
       <c r="E86" s="7">
         <v>1</v>
@@ -5809,7 +6034,7 @@
         <v>413</v>
       </c>
       <c r="D87" t="s">
-        <v>462</v>
+        <v>481</v>
       </c>
       <c r="E87" s="7">
         <v>1</v>
@@ -5853,7 +6078,7 @@
         <v>414</v>
       </c>
       <c r="D88" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="E88" s="7">
         <v>1</v>
@@ -5897,7 +6122,7 @@
         <v>415</v>
       </c>
       <c r="D89" t="s">
-        <v>462</v>
+        <v>483</v>
       </c>
       <c r="E89" s="7">
         <v>1</v>
@@ -5941,7 +6166,7 @@
         <v>416</v>
       </c>
       <c r="D90" t="s">
-        <v>462</v>
+        <v>484</v>
       </c>
       <c r="E90" s="7">
         <v>1</v>
@@ -5985,7 +6210,7 @@
         <v>417</v>
       </c>
       <c r="D91" t="s">
-        <v>462</v>
+        <v>485</v>
       </c>
       <c r="E91" s="7">
         <v>1</v>
@@ -6029,7 +6254,7 @@
         <v>418</v>
       </c>
       <c r="D92" t="s">
-        <v>462</v>
+        <v>486</v>
       </c>
       <c r="E92" s="7">
         <v>1</v>
@@ -6073,7 +6298,7 @@
         <v>419</v>
       </c>
       <c r="D93" t="s">
-        <v>462</v>
+        <v>487</v>
       </c>
       <c r="E93" s="7">
         <v>1</v>
@@ -6117,7 +6342,7 @@
         <v>420</v>
       </c>
       <c r="D94" t="s">
-        <v>462</v>
+        <v>488</v>
       </c>
       <c r="E94" s="7">
         <v>1</v>
@@ -6161,7 +6386,7 @@
         <v>421</v>
       </c>
       <c r="D95" t="s">
-        <v>462</v>
+        <v>489</v>
       </c>
       <c r="E95" s="7">
         <v>1</v>
@@ -6205,7 +6430,7 @@
         <v>422</v>
       </c>
       <c r="D96" t="s">
-        <v>462</v>
+        <v>489</v>
       </c>
       <c r="E96" s="7">
         <v>1</v>
@@ -6249,7 +6474,7 @@
         <v>423</v>
       </c>
       <c r="D97" t="s">
-        <v>462</v>
+        <v>490</v>
       </c>
       <c r="E97" s="7">
         <v>1</v>
@@ -6293,7 +6518,7 @@
         <v>424</v>
       </c>
       <c r="D98" t="s">
-        <v>462</v>
+        <v>491</v>
       </c>
       <c r="E98" s="7">
         <v>1</v>
@@ -6331,7 +6556,7 @@
         <v>425</v>
       </c>
       <c r="D99" t="s">
-        <v>462</v>
+        <v>491</v>
       </c>
       <c r="E99" s="7">
         <v>1</v>
@@ -6375,7 +6600,7 @@
         <v>426</v>
       </c>
       <c r="D100" t="s">
-        <v>462</v>
+        <v>492</v>
       </c>
       <c r="E100" s="7">
         <v>1</v>
@@ -6419,7 +6644,7 @@
         <v>427</v>
       </c>
       <c r="D101" t="s">
-        <v>462</v>
+        <v>492</v>
       </c>
       <c r="E101" s="7">
         <v>1</v>
@@ -6463,10 +6688,10 @@
         <v>428</v>
       </c>
       <c r="D102" t="s">
-        <v>462</v>
+        <v>492</v>
       </c>
       <c r="E102" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F102" s="6" t="s">
         <v>13</v>
@@ -6507,7 +6732,7 @@
         <v>429</v>
       </c>
       <c r="D103" t="s">
-        <v>462</v>
+        <v>493</v>
       </c>
       <c r="E103" s="7">
         <v>1</v>
@@ -6551,7 +6776,7 @@
         <v>430</v>
       </c>
       <c r="D104" t="s">
-        <v>462</v>
+        <v>493</v>
       </c>
       <c r="E104" s="7">
         <v>1</v>
@@ -6595,7 +6820,7 @@
         <v>431</v>
       </c>
       <c r="D105" t="s">
-        <v>462</v>
+        <v>494</v>
       </c>
       <c r="E105" s="7">
         <v>1</v>
@@ -6639,7 +6864,7 @@
         <v>432</v>
       </c>
       <c r="D106" t="s">
-        <v>462</v>
+        <v>494</v>
       </c>
       <c r="E106" s="7">
         <v>1</v>
@@ -6683,7 +6908,7 @@
         <v>433</v>
       </c>
       <c r="D107" t="s">
-        <v>462</v>
+        <v>494</v>
       </c>
       <c r="E107" s="7">
         <v>1</v>
@@ -6727,7 +6952,7 @@
         <v>434</v>
       </c>
       <c r="D108" t="s">
-        <v>462</v>
+        <v>495</v>
       </c>
       <c r="E108" s="7">
         <v>1</v>
@@ -6771,7 +6996,7 @@
         <v>435</v>
       </c>
       <c r="D109" t="s">
-        <v>462</v>
+        <v>496</v>
       </c>
       <c r="E109" s="7">
         <v>1</v>
@@ -6815,7 +7040,7 @@
         <v>436</v>
       </c>
       <c r="D110" t="s">
-        <v>462</v>
+        <v>497</v>
       </c>
       <c r="E110" s="7">
         <v>1</v>
@@ -6859,7 +7084,7 @@
         <v>437</v>
       </c>
       <c r="D111" t="s">
-        <v>462</v>
+        <v>498</v>
       </c>
       <c r="E111" s="7">
         <v>1</v>
@@ -6903,7 +7128,7 @@
         <v>438</v>
       </c>
       <c r="D112" t="s">
-        <v>462</v>
+        <v>499</v>
       </c>
       <c r="E112" s="7">
         <v>1</v>
@@ -6947,7 +7172,7 @@
         <v>439</v>
       </c>
       <c r="D113" t="s">
-        <v>462</v>
+        <v>499</v>
       </c>
       <c r="E113" s="7">
         <v>1</v>
@@ -6991,7 +7216,7 @@
         <v>440</v>
       </c>
       <c r="D114" t="s">
-        <v>462</v>
+        <v>499</v>
       </c>
       <c r="E114" s="7">
         <v>1</v>
@@ -7035,7 +7260,7 @@
         <v>441</v>
       </c>
       <c r="D115" t="s">
-        <v>462</v>
+        <v>500</v>
       </c>
       <c r="E115" s="7">
         <v>1</v>
@@ -7079,7 +7304,7 @@
         <v>442</v>
       </c>
       <c r="D116" t="s">
-        <v>462</v>
+        <v>501</v>
       </c>
       <c r="E116" s="7">
         <v>1</v>
@@ -7123,7 +7348,7 @@
         <v>443</v>
       </c>
       <c r="D117" t="s">
-        <v>462</v>
+        <v>502</v>
       </c>
       <c r="E117" s="7">
         <v>1</v>
@@ -7167,7 +7392,7 @@
         <v>444</v>
       </c>
       <c r="D118" t="s">
-        <v>462</v>
+        <v>502</v>
       </c>
       <c r="E118" s="7">
         <v>1</v>
@@ -7211,7 +7436,7 @@
         <v>445</v>
       </c>
       <c r="D119" t="s">
-        <v>462</v>
+        <v>502</v>
       </c>
       <c r="E119" s="7">
         <v>2</v>
@@ -7255,7 +7480,7 @@
         <v>446</v>
       </c>
       <c r="D120" t="s">
-        <v>462</v>
+        <v>503</v>
       </c>
       <c r="E120" s="7">
         <v>1</v>
@@ -7299,7 +7524,7 @@
         <v>447</v>
       </c>
       <c r="D121" t="s">
-        <v>462</v>
+        <v>504</v>
       </c>
       <c r="E121" s="7">
         <v>1</v>
@@ -7343,7 +7568,7 @@
         <v>448</v>
       </c>
       <c r="D122" t="s">
-        <v>462</v>
+        <v>504</v>
       </c>
       <c r="E122" s="7">
         <v>1</v>
@@ -7387,7 +7612,7 @@
         <v>449</v>
       </c>
       <c r="D123" t="s">
-        <v>462</v>
+        <v>505</v>
       </c>
       <c r="E123" s="7">
         <v>1</v>
@@ -7431,7 +7656,7 @@
         <v>450</v>
       </c>
       <c r="D124" t="s">
-        <v>462</v>
+        <v>506</v>
       </c>
       <c r="E124" s="7">
         <v>1</v>
@@ -7475,7 +7700,7 @@
         <v>451</v>
       </c>
       <c r="D125" t="s">
-        <v>462</v>
+        <v>507</v>
       </c>
       <c r="E125" s="7">
         <v>1</v>
@@ -7519,7 +7744,7 @@
         <v>452</v>
       </c>
       <c r="D126" t="s">
-        <v>462</v>
+        <v>507</v>
       </c>
       <c r="E126" s="7">
         <v>1</v>
@@ -7563,7 +7788,7 @@
         <v>453</v>
       </c>
       <c r="D127" t="s">
-        <v>462</v>
+        <v>508</v>
       </c>
       <c r="E127" s="7">
         <v>1</v>
@@ -7607,7 +7832,7 @@
         <v>454</v>
       </c>
       <c r="D128" t="s">
-        <v>462</v>
+        <v>509</v>
       </c>
       <c r="E128" s="7">
         <v>1</v>
@@ -7651,7 +7876,7 @@
         <v>455</v>
       </c>
       <c r="D129" t="s">
-        <v>462</v>
+        <v>510</v>
       </c>
       <c r="E129" s="7">
         <v>1</v>
@@ -7695,7 +7920,7 @@
         <v>456</v>
       </c>
       <c r="D130" t="s">
-        <v>462</v>
+        <v>511</v>
       </c>
       <c r="E130" s="7">
         <v>1</v>
@@ -7739,7 +7964,7 @@
         <v>457</v>
       </c>
       <c r="D131" t="s">
-        <v>462</v>
+        <v>512</v>
       </c>
       <c r="E131" s="7">
         <v>1</v>
@@ -7783,7 +8008,7 @@
         <v>458</v>
       </c>
       <c r="D132" t="s">
-        <v>462</v>
+        <v>512</v>
       </c>
       <c r="E132" s="7">
         <v>1</v>
@@ -7827,7 +8052,7 @@
         <v>459</v>
       </c>
       <c r="D133" t="s">
-        <v>462</v>
+        <v>513</v>
       </c>
       <c r="E133" s="7">
         <v>1</v>
@@ -7871,7 +8096,7 @@
         <v>460</v>
       </c>
       <c r="D134" t="s">
-        <v>462</v>
+        <v>514</v>
       </c>
       <c r="E134" s="7">
         <v>1</v>
@@ -7915,7 +8140,7 @@
         <v>461</v>
       </c>
       <c r="D135" t="s">
-        <v>462</v>
+        <v>515</v>
       </c>
       <c r="E135" s="7">
         <v>1</v>
@@ -7959,7 +8184,7 @@
         <v>325</v>
       </c>
       <c r="D136" t="s">
-        <v>462</v>
+        <v>516</v>
       </c>
       <c r="E136" s="7">
         <v>1</v>
@@ -8003,7 +8228,7 @@
         <v>328</v>
       </c>
       <c r="D137" t="s">
-        <v>462</v>
+        <v>517</v>
       </c>
       <c r="E137" s="7">
         <v>1</v>
@@ -8047,7 +8272,7 @@
         <v>330</v>
       </c>
       <c r="D138" t="s">
-        <v>462</v>
+        <v>518</v>
       </c>
       <c r="E138" s="7">
         <v>1</v>
@@ -8091,7 +8316,7 @@
         <v>332</v>
       </c>
       <c r="D139" t="s">
-        <v>462</v>
+        <v>519</v>
       </c>
       <c r="E139" s="7">
         <v>1</v>
@@ -8135,7 +8360,7 @@
         <v>334</v>
       </c>
       <c r="D140" t="s">
-        <v>462</v>
+        <v>520</v>
       </c>
       <c r="E140" s="7">
         <v>1</v>
@@ -8179,7 +8404,7 @@
         <v>335</v>
       </c>
       <c r="D141" t="s">
-        <v>462</v>
+        <v>520</v>
       </c>
       <c r="E141" s="7">
         <v>1</v>
@@ -8223,7 +8448,7 @@
         <v>336</v>
       </c>
       <c r="D142" t="s">
-        <v>462</v>
+        <v>520</v>
       </c>
       <c r="E142" s="7">
         <v>1</v>
@@ -8267,7 +8492,7 @@
         <v>338</v>
       </c>
       <c r="D143" t="s">
-        <v>462</v>
+        <v>521</v>
       </c>
       <c r="E143" s="7">
         <v>1</v>
@@ -8311,7 +8536,7 @@
         <v>339</v>
       </c>
       <c r="D144" t="s">
-        <v>462</v>
+        <v>521</v>
       </c>
       <c r="E144" s="7">
         <v>1</v>
@@ -8355,7 +8580,7 @@
         <v>340</v>
       </c>
       <c r="D145" t="s">
-        <v>462</v>
+        <v>521</v>
       </c>
       <c r="E145" s="7">
         <v>1</v>
@@ -8399,7 +8624,7 @@
         <v>342</v>
       </c>
       <c r="D146" t="s">
-        <v>462</v>
+        <v>522</v>
       </c>
       <c r="E146" s="7">
         <v>1</v>
@@ -8443,7 +8668,7 @@
         <v>344</v>
       </c>
       <c r="D147" t="s">
-        <v>462</v>
+        <v>523</v>
       </c>
       <c r="E147" s="7">
         <v>1</v>
@@ -8487,7 +8712,7 @@
         <v>345</v>
       </c>
       <c r="D148" t="s">
-        <v>462</v>
+        <v>523</v>
       </c>
       <c r="E148" s="7">
         <v>1</v>
@@ -8531,7 +8756,7 @@
         <v>346</v>
       </c>
       <c r="D149" t="s">
-        <v>462</v>
+        <v>523</v>
       </c>
       <c r="E149" s="7">
         <v>1</v>
@@ -8575,7 +8800,7 @@
         <v>348</v>
       </c>
       <c r="D150" t="s">
-        <v>462</v>
+        <v>524</v>
       </c>
       <c r="E150" s="7">
         <v>1</v>
@@ -8619,7 +8844,7 @@
         <v>350</v>
       </c>
       <c r="D151" t="s">
-        <v>462</v>
+        <v>525</v>
       </c>
       <c r="E151" s="7">
         <v>1</v>
@@ -8663,7 +8888,7 @@
         <v>351</v>
       </c>
       <c r="D152" t="s">
-        <v>462</v>
+        <v>525</v>
       </c>
       <c r="E152" s="7">
         <v>1</v>
@@ -8707,7 +8932,7 @@
         <v>352</v>
       </c>
       <c r="D153" t="s">
-        <v>462</v>
+        <v>525</v>
       </c>
       <c r="E153" s="7">
         <v>1</v>
@@ -8751,7 +8976,7 @@
         <v>354</v>
       </c>
       <c r="D154" t="s">
-        <v>462</v>
+        <v>526</v>
       </c>
       <c r="E154" s="7">
         <v>1</v>
@@ -8795,7 +9020,7 @@
         <v>355</v>
       </c>
       <c r="D155" t="s">
-        <v>462</v>
+        <v>526</v>
       </c>
       <c r="E155" s="7">
         <v>1</v>
@@ -8839,7 +9064,7 @@
         <v>356</v>
       </c>
       <c r="D156" t="s">
-        <v>462</v>
+        <v>526</v>
       </c>
       <c r="E156" s="7">
         <v>1</v>
@@ -8883,7 +9108,7 @@
         <v>358</v>
       </c>
       <c r="D157" t="s">
-        <v>462</v>
+        <v>527</v>
       </c>
       <c r="E157" s="7">
         <v>1</v>
@@ -8927,7 +9152,7 @@
         <v>360</v>
       </c>
       <c r="D158" t="s">
-        <v>462</v>
+        <v>528</v>
       </c>
       <c r="E158" s="7">
         <v>1</v>
@@ -8971,7 +9196,7 @@
         <v>362</v>
       </c>
       <c r="D159" t="s">
-        <v>462</v>
+        <v>529</v>
       </c>
       <c r="E159" s="7">
         <v>1</v>
@@ -9015,7 +9240,7 @@
         <v>364</v>
       </c>
       <c r="D160" t="s">
-        <v>462</v>
+        <v>530</v>
       </c>
       <c r="E160" s="7">
         <v>1</v>
@@ -9059,7 +9284,7 @@
         <v>365</v>
       </c>
       <c r="D161" t="s">
-        <v>462</v>
+        <v>530</v>
       </c>
       <c r="E161" s="7">
         <v>1</v>
@@ -9103,7 +9328,7 @@
         <v>366</v>
       </c>
       <c r="D162" t="s">
-        <v>462</v>
+        <v>530</v>
       </c>
       <c r="E162" s="7">
         <v>1</v>
@@ -9147,7 +9372,7 @@
         <v>367</v>
       </c>
       <c r="D163" t="s">
-        <v>462</v>
+        <v>530</v>
       </c>
       <c r="E163" s="7">
         <v>1</v>
@@ -9191,7 +9416,7 @@
         <v>368</v>
       </c>
       <c r="D164" t="s">
-        <v>462</v>
+        <v>530</v>
       </c>
       <c r="E164" s="7">
         <v>1</v>
@@ -9235,7 +9460,7 @@
         <v>370</v>
       </c>
       <c r="D165" t="s">
-        <v>462</v>
+        <v>531</v>
       </c>
       <c r="E165" s="7">
         <v>1</v>
@@ -9279,7 +9504,7 @@
         <v>372</v>
       </c>
       <c r="D166" t="s">
-        <v>462</v>
+        <v>532</v>
       </c>
       <c r="E166" s="7">
         <v>1</v>
@@ -9323,7 +9548,7 @@
         <v>374</v>
       </c>
       <c r="D167" t="s">
-        <v>462</v>
+        <v>533</v>
       </c>
       <c r="E167" s="7">
         <v>1</v>
@@ -9367,7 +9592,7 @@
         <v>377</v>
       </c>
       <c r="D168" t="s">
-        <v>462</v>
+        <v>534</v>
       </c>
       <c r="E168" s="7">
         <v>1</v>
@@ -9411,7 +9636,7 @@
         <v>379</v>
       </c>
       <c r="D169" t="s">
-        <v>462</v>
+        <v>535</v>
       </c>
       <c r="E169" s="7">
         <v>1</v>
@@ -9455,7 +9680,7 @@
         <v>381</v>
       </c>
       <c r="D170" t="s">
-        <v>462</v>
+        <v>536</v>
       </c>
       <c r="E170" s="7">
         <v>1</v>
@@ -9499,7 +9724,7 @@
         <v>383</v>
       </c>
       <c r="D171" t="s">
-        <v>462</v>
+        <v>536</v>
       </c>
       <c r="E171" s="7">
         <v>1</v>
@@ -9543,7 +9768,7 @@
         <v>384</v>
       </c>
       <c r="D172" t="s">
-        <v>462</v>
+        <v>536</v>
       </c>
       <c r="E172" s="7">
         <v>1</v>
@@ -9587,7 +9812,7 @@
         <v>386</v>
       </c>
       <c r="D173" t="s">
-        <v>462</v>
+        <v>537</v>
       </c>
       <c r="E173" s="7">
         <v>1</v>

</xml_diff>

<commit_message>
Fix a missing information in CardPoolDatabase.xlsx for CID=96 "Ballista".
</commit_message>
<xml_diff>
--- a/Resources/CardPoolDatabase.xlsx
+++ b/Resources/CardPoolDatabase.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cpp\GwentCore\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Junce\Source\Repos\GwentCore\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1734" uniqueCount="537">
   <si>
     <t>Name</t>
   </si>
@@ -2215,8 +2215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q173"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6529,15 +6529,21 @@
       <c r="H98" s="6">
         <v>6</v>
       </c>
-      <c r="I98" s="6"/>
-      <c r="J98" s="6"/>
+      <c r="I98" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J98" s="6" t="s">
+        <v>222</v>
+      </c>
       <c r="K98" s="6" t="s">
         <v>306</v>
       </c>
       <c r="L98" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="M98" s="6"/>
+      <c r="M98" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="N98" s="4" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
A better version for database
</commit_message>
<xml_diff>
--- a/Resources/CardPoolDatabase.xlsx
+++ b/Resources/CardPoolDatabase.xlsx
@@ -2211,8 +2211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>